<commit_message>
NetworkX implementation and clean-up
</commit_message>
<xml_diff>
--- a/nile_EMODPS_framework/settings/settings_file_Nile.xlsx
+++ b/nile_EMODPS_framework/settings/settings_file_Nile.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yasinsari/Documents/master-thesis-project/nile_EMODPS_framework/settings/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yasinsari/Documents/eastern-nile-optimization/nile_EMODPS_framework/settings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05377291-8EAC-BA42-B8ED-350E1574D52C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3547360-BE2F-7546-97BD-4CEA559C33F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27860" yWindow="3400" windowWidth="27860" windowHeight="15580" activeTab="1" xr2:uid="{65B2DD87-E74E-094B-8E0A-FAA834E63631}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" xr2:uid="{65B2DD87-E74E-094B-8E0A-FAA834E63631}"/>
   </bookViews>
   <sheets>
-    <sheet name="ModelParameters" sheetId="4" r:id="rId1"/>
-    <sheet name="Reservoirs" sheetId="1" r:id="rId2"/>
-    <sheet name="PolicyParameters" sheetId="5" r:id="rId3"/>
+    <sheet name="Topology" sheetId="6" r:id="rId1"/>
+    <sheet name="ModelParameters" sheetId="4" r:id="rId2"/>
+    <sheet name="ReservoirParameters" sheetId="1" r:id="rId3"/>
+    <sheet name="PolicyParameters" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="93">
   <si>
     <t>Simulation Horizon</t>
   </si>
@@ -108,9 +109,6 @@
     <t>Initial Storage(m3)</t>
   </si>
   <si>
-    <t>Hydroelectric Turbine Count</t>
-  </si>
-  <si>
     <t>Max Turbine Flow</t>
   </si>
   <si>
@@ -228,48 +226,9 @@
     <t>["USSennar", "Gezira", "DSSennar", "Taminiat", "Hassanab", "Egypt"]</t>
   </si>
   <si>
-    <t>[467]</t>
-  </si>
-  <si>
-    <t>[417.2]</t>
-  </si>
-  <si>
-    <t>[147]</t>
-  </si>
-  <si>
     <t>Max Capacity</t>
   </si>
   <si>
-    <t>[6000]</t>
-  </si>
-  <si>
-    <t>[280]</t>
-  </si>
-  <si>
-    <t>[15]</t>
-  </si>
-  <si>
-    <t>[2100]</t>
-  </si>
-  <si>
-    <t>[117]</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>[4211]</t>
-  </si>
-  <si>
-    <t>[1031.65]</t>
-  </si>
-  <si>
-    <t>[0.90]</t>
-  </si>
-  <si>
-    <t>[0.60]</t>
-  </si>
-  <si>
     <t>[0,0,0, 0,1,0]</t>
   </si>
   <si>
@@ -285,50 +244,92 @@
     <t>Roseires</t>
   </si>
   <si>
-    <t>Filling Time of GERD</t>
-  </si>
-  <si>
-    <t>years</t>
-  </si>
-  <si>
-    <t>GERD_filling_time</t>
-  </si>
-  <si>
     <t>half-an-hour</t>
   </si>
   <si>
-    <t>[0.93]</t>
-  </si>
-  <si>
-    <t>[4320]</t>
-  </si>
-  <si>
-    <t>[507]</t>
+    <t>Network ID</t>
+  </si>
+  <si>
+    <t>Catchment</t>
+  </si>
+  <si>
+    <t>BlueNile</t>
+  </si>
+  <si>
+    <t>Outgoing Nodes</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Reservoir</t>
+  </si>
+  <si>
+    <t>GERDToRoseires</t>
+  </si>
+  <si>
+    <t>RoseiresToAbuNaama</t>
+  </si>
+  <si>
+    <t>USSennar</t>
+  </si>
+  <si>
+    <t>SukiToSennar</t>
+  </si>
+  <si>
+    <t>Gezira</t>
+  </si>
+  <si>
+    <t>Dinder</t>
+  </si>
+  <si>
+    <t>Rahad</t>
+  </si>
+  <si>
+    <t>DSSennar</t>
+  </si>
+  <si>
+    <t>WhiteNile</t>
+  </si>
+  <si>
+    <t>Tamaniat</t>
+  </si>
+  <si>
+    <t>Atbara</t>
+  </si>
+  <si>
+    <t>Hassanab</t>
+  </si>
+  <si>
+    <t>Egypt</t>
+  </si>
+  <si>
+    <t>IrrigationDistrict</t>
+  </si>
+  <si>
+    <t>Delay</t>
+  </si>
+  <si>
+    <t>Hydropower Exists</t>
+  </si>
+  <si>
+    <t>Initial for Delay</t>
+  </si>
+  <si>
+    <t>[934.2]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFD4D4D4"/>
-      <name val="Menlo"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF569CD6"/>
-      <name val="Menlo"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -355,12 +356,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -368,6 +363,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -384,18 +385,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -709,35 +709,387 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88C088A8-03D6-1140-857A-EC8C8A0D1928}">
+  <dimension ref="A1:F19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="153" zoomScaleNormal="153" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.5" customWidth="1"/>
+    <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C7" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7">
+        <v>6</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8" t="s">
+        <v>78</v>
+      </c>
+      <c r="D8">
+        <v>7</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D9">
+        <v>8</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>88</v>
+      </c>
+      <c r="C10" t="s">
+        <v>79</v>
+      </c>
+      <c r="D10">
+        <v>9</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" t="s">
+        <v>80</v>
+      </c>
+      <c r="D11">
+        <v>10</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>70</v>
+      </c>
+      <c r="C12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D12">
+        <v>11</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>88</v>
+      </c>
+      <c r="C13" t="s">
+        <v>82</v>
+      </c>
+      <c r="D13">
+        <v>12</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>70</v>
+      </c>
+      <c r="C14" t="s">
+        <v>83</v>
+      </c>
+      <c r="D14">
+        <v>13</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>88</v>
+      </c>
+      <c r="C15" t="s">
+        <v>84</v>
+      </c>
+      <c r="D15">
+        <v>14</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16" t="s">
+        <v>85</v>
+      </c>
+      <c r="D16">
+        <v>15</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>88</v>
+      </c>
+      <c r="C17" t="s">
+        <v>86</v>
+      </c>
+      <c r="D17">
+        <v>16</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>74</v>
+      </c>
+      <c r="C18" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18">
+        <v>17</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>88</v>
+      </c>
+      <c r="C19" t="s">
+        <v>87</v>
+      </c>
+      <c r="D19" t="s">
+        <v>73</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10871A19-541A-E94D-BB27-74C5363B6884}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView zoomScale="157" zoomScaleNormal="157" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="65.33203125" customWidth="1"/>
+    <col min="2" max="2" width="61.6640625" customWidth="1"/>
     <col min="3" max="3" width="11.33203125" customWidth="1"/>
     <col min="4" max="4" width="20.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -779,7 +1131,7 @@
       <c r="A4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="3">
         <v>1441.99</v>
       </c>
       <c r="C4" t="s">
@@ -810,377 +1162,72 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="A6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B6" t="s">
+      <c r="E6" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C8" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" t="s">
-        <v>80</v>
-      </c>
-      <c r="C7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="D8" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="7" t="s">
         <v>28</v>
-      </c>
-      <c r="E7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B8" t="s">
-        <v>62</v>
-      </c>
-      <c r="C8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B9" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
       <c r="C9" t="s">
         <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>82</v>
-      </c>
-      <c r="B10">
-        <v>5</v>
-      </c>
-      <c r="C10" t="s">
-        <v>83</v>
-      </c>
-      <c r="D10" t="s">
-        <v>84</v>
-      </c>
-      <c r="E10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C46D96C-8ADA-8E40-B2A8-24351E5FCFAE}">
-  <dimension ref="A1:N57"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="24" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" customWidth="1"/>
-    <col min="7" max="7" width="13" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B2" s="10">
-        <v>15000000000</v>
-      </c>
-      <c r="C2" s="5">
-        <v>1</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>81</v>
-      </c>
-      <c r="B3" s="6">
-        <v>4571250000</v>
-      </c>
-      <c r="C3" s="5">
-        <v>1</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B4" s="6">
-        <v>434925000</v>
-      </c>
-      <c r="C4" s="5">
-        <v>1</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>60</v>
-      </c>
-      <c r="B5" s="6">
-        <v>137025000000</v>
-      </c>
-      <c r="C5" s="5">
-        <v>1</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F15" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="22" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C22" s="2"/>
-      <c r="N22" s="2"/>
-    </row>
-    <row r="23" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C23" s="1"/>
-      <c r="N23" s="1"/>
-    </row>
-    <row r="24" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C24" s="2"/>
-      <c r="N24" s="2"/>
-    </row>
-    <row r="25" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C25" s="1"/>
-      <c r="N25" s="1"/>
-    </row>
-    <row r="26" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C26" s="2"/>
-      <c r="N26" s="2"/>
-    </row>
-    <row r="27" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C27" s="1"/>
-      <c r="N27" s="1"/>
-    </row>
-    <row r="28" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C28" s="2"/>
-      <c r="N28" s="2"/>
-    </row>
-    <row r="29" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C29" s="1"/>
-      <c r="N29" s="1"/>
-    </row>
-    <row r="30" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C30" s="2"/>
-      <c r="N30" s="2"/>
-    </row>
-    <row r="31" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C31" s="1"/>
-      <c r="N31" s="1"/>
-    </row>
-    <row r="32" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C32" s="2"/>
-      <c r="N32" s="2"/>
-    </row>
-    <row r="33" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C33" s="1"/>
-      <c r="N33" s="1"/>
-    </row>
-    <row r="34" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C34" s="2"/>
-      <c r="N34" s="2"/>
-    </row>
-    <row r="35" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C35" s="1"/>
-      <c r="N35" s="1"/>
-    </row>
-    <row r="36" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C36" s="2"/>
-      <c r="N36" s="2"/>
-    </row>
-    <row r="37" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C37" s="1"/>
-      <c r="N37" s="1"/>
-    </row>
-    <row r="38" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C38" s="2"/>
-      <c r="N38" s="2"/>
-    </row>
-    <row r="39" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C39" s="1"/>
-      <c r="N39" s="1"/>
-    </row>
-    <row r="40" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C40" s="2"/>
-      <c r="N40" s="2"/>
-    </row>
-    <row r="41" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C41" s="1"/>
-      <c r="N41" s="1"/>
-    </row>
-    <row r="42" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C42" s="2"/>
-      <c r="N42" s="2"/>
-    </row>
-    <row r="43" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C43" s="1"/>
-      <c r="N43" s="1"/>
-    </row>
-    <row r="44" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C44" s="2"/>
-      <c r="N44" s="2"/>
-    </row>
-    <row r="45" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C45" s="1"/>
-      <c r="N45" s="1"/>
-    </row>
-    <row r="46" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C46" s="2"/>
-      <c r="N46" s="2"/>
-    </row>
-    <row r="47" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C47" s="1"/>
-      <c r="N47" s="1"/>
-    </row>
-    <row r="48" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C48" s="2"/>
-      <c r="N48" s="2"/>
-    </row>
-    <row r="49" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C49" s="1"/>
-      <c r="N49" s="1"/>
-    </row>
-    <row r="50" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C50" s="2"/>
-      <c r="N50" s="2"/>
-    </row>
-    <row r="51" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C51" s="1"/>
-      <c r="N51" s="1"/>
-    </row>
-    <row r="52" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C52" s="2"/>
-      <c r="N52" s="2"/>
-    </row>
-    <row r="53" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C53" s="1"/>
-      <c r="N53" s="1"/>
-    </row>
-    <row r="54" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C54" s="2"/>
-      <c r="N54" s="2"/>
-    </row>
-    <row r="55" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C55" s="1"/>
-      <c r="N55" s="1"/>
-    </row>
-    <row r="56" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C56" s="2"/>
-      <c r="N56" s="2"/>
-    </row>
-    <row r="57" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C57" s="1"/>
-      <c r="N57" s="1"/>
+        <v>52</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1188,6 +1235,144 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C46D96C-8ADA-8E40-B2A8-24351E5FCFAE}">
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="19.1640625" customWidth="1"/>
+    <col min="4" max="4" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="6" max="6" width="15.1640625" customWidth="1"/>
+    <col min="7" max="7" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="8">
+        <v>15000000000</v>
+      </c>
+      <c r="C2" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" s="9">
+        <v>4320</v>
+      </c>
+      <c r="E2" s="9">
+        <v>0.93</v>
+      </c>
+      <c r="F2" s="9">
+        <v>507</v>
+      </c>
+      <c r="G2" s="9">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" s="9">
+        <v>4571250000</v>
+      </c>
+      <c r="C3" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D3" s="9">
+        <v>1031.6500000000001</v>
+      </c>
+      <c r="E3" s="9">
+        <v>0.6</v>
+      </c>
+      <c r="F3" s="9">
+        <v>467</v>
+      </c>
+      <c r="G3" s="9">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" s="9">
+        <v>434925000</v>
+      </c>
+      <c r="C4" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D4" s="9">
+        <v>117</v>
+      </c>
+      <c r="E4" s="9">
+        <v>0.6</v>
+      </c>
+      <c r="F4" s="9">
+        <v>417.2</v>
+      </c>
+      <c r="G4" s="9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="9">
+        <v>137025000000</v>
+      </c>
+      <c r="C5" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D5" s="9">
+        <v>4211</v>
+      </c>
+      <c r="E5" s="9">
+        <v>0.9</v>
+      </c>
+      <c r="F5" s="9">
+        <v>147</v>
+      </c>
+      <c r="G5" s="9">
+        <v>2100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22103061-AE41-8A4B-969C-CFE2C42F73B9}">
   <dimension ref="A1:E14"/>
   <sheetViews>
@@ -1204,73 +1389,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="B4" s="5">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
         <v>45</v>
-      </c>
-      <c r="E2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="8">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>46</v>
       </c>
       <c r="E4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B5" s="8">
+      <c r="A5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="5">
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E5" t="s">
         <v>7</v>
@@ -1278,13 +1463,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B6" s="8">
+        <v>42</v>
+      </c>
+      <c r="B6" s="5">
         <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E6" t="s">
         <v>7</v>
@@ -1292,13 +1477,13 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>78</v>
+        <v>36</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>64</v>
       </c>
       <c r="D7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E7" t="s">
         <v>20</v>
@@ -1306,13 +1491,13 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>38</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>79</v>
+        <v>37</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>65</v>
       </c>
       <c r="D8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E8" t="s">
         <v>20</v>
@@ -1320,13 +1505,13 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>77</v>
+        <v>38</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>63</v>
       </c>
       <c r="D9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E9" t="s">
         <v>20</v>
@@ -1334,29 +1519,29 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>40</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>55</v>
+        <v>39</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>54</v>
       </c>
       <c r="D10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E10" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="4"/>
+      <c r="A11" s="2"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="4"/>
+      <c r="A12" s="2"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="4"/>
+      <c r="A13" s="2"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="4"/>
+      <c r="A14" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>